<commit_message>
Add some fields needed for reporting
</commit_message>
<xml_diff>
--- a/Configs/FRTBConfig_EU-EBA.xlsx
+++ b/Configs/FRTBConfig_EU-EBA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alan/Workspace/FRTB/Configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC02F982-6A9C-7340-82EC-AA58F63B4085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7077843F-9A3A-C845-BE7C-ABD2ADA3D89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="79560" yWindow="10580" windowWidth="39620" windowHeight="26960" activeTab="11" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
+    <workbookView xWindow="79560" yWindow="10580" windowWidth="39620" windowHeight="26960" xr2:uid="{702274BA-38C3-0147-8564-8B67C0FD49FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Copyright" sheetId="23" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="353">
   <si>
     <t>Bucket</t>
   </si>
@@ -1187,6 +1187,9 @@
   </si>
   <si>
     <t>Others</t>
+  </si>
+  <si>
+    <t>In the EU, buckets 3, 3a and 3b have separately specified risk weights but are the same buket for intra- and inter- bucket computations.</t>
   </si>
 </sst>
 </file>
@@ -1678,7 +1681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{896FB02E-B9E7-EE44-B543-FBA941EB6786}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2000,7 +2003,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -15494,10 +15497,13 @@
         <v>10</v>
       </c>
     </row>
+    <row r="35" spans="4:4">
+      <c r="D35" t="s">
+        <v>352</v>
+      </c>
+    </row>
     <row r="42" spans="4:4">
-      <c r="D42" s="20" t="s">
-        <v>310</v>
-      </c>
+      <c r="D42" s="20"/>
     </row>
     <row r="43" spans="4:4">
       <c r="D43" s="20"/>

</xml_diff>